<commit_message>
Input data from Sept and new plots of raw data
Plot pie charts of coarse/fine in tubes and pods by month from the LAB
sheet
</commit_message>
<xml_diff>
--- a/Data/BulkWeight/SedPod_Processing_LAB.xlsx
+++ b/Data/BulkWeight/SedPod_Processing_LAB.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Apr" sheetId="1" r:id="rId1"/>
-    <sheet name="May-Jun" sheetId="5" r:id="rId2"/>
-    <sheet name="Jul" sheetId="4" r:id="rId3"/>
-    <sheet name="Aug" sheetId="6" r:id="rId4"/>
+    <sheet name="Mar" sheetId="1" r:id="rId1"/>
+    <sheet name="April" sheetId="5" r:id="rId2"/>
+    <sheet name="May" sheetId="4" r:id="rId3"/>
+    <sheet name="Jun_Jul" sheetId="6" r:id="rId4"/>
     <sheet name="Aug_Sept" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="55">
   <si>
     <t>Pod(P)/Tube(T)</t>
   </si>
@@ -93,18 +93,12 @@
     <t>Date of Processing:</t>
   </si>
   <si>
-    <t>August/September 2014</t>
-  </si>
-  <si>
     <t>Messina</t>
   </si>
   <si>
     <t xml:space="preserve">SedPod/SedTube Processing </t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Newtson</t>
   </si>
   <si>
@@ -181,13 +175,31 @@
   </si>
   <si>
     <t>T2A-5</t>
+  </si>
+  <si>
+    <t>P1Ca</t>
+  </si>
+  <si>
+    <t>P2Aa</t>
+  </si>
+  <si>
+    <t>Oven Start:</t>
+  </si>
+  <si>
+    <t>Oven End:</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>Lon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -207,6 +219,14 @@
       <b/>
       <i/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -297,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -312,9 +332,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -322,31 +339,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -712,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -730,25 +732,28 @@
     <col min="8" max="8" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="9">
+        <v>41703</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="9">
+        <v>41740</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -756,30 +761,30 @@
         <v>41772</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="F7" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="F7" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -792,7 +797,7 @@
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="5" t="s">
         <v>1</v>
       </c>
@@ -802,10 +807,16 @@
       <c r="H8" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1">
         <v>69.311999999999998</v>
@@ -817,7 +828,7 @@
         <f>C9-B9</f>
         <v>7.2169999999999987</v>
       </c>
-      <c r="E9" s="16"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="6">
         <v>1.7410000000000001</v>
       </c>
@@ -828,10 +839,16 @@
         <f>G9-F9</f>
         <v>0.52099999999999991</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>-14.290179999999999</v>
+      </c>
+      <c r="J9">
+        <v>-170.6814</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1">
         <v>70.331999999999994</v>
@@ -843,7 +860,7 @@
         <f>C10-B10</f>
         <v>2.2420000000000044</v>
       </c>
-      <c r="E10" s="16"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="6">
         <v>1.7450000000000001</v>
       </c>
@@ -854,10 +871,16 @@
         <f>G10-F10</f>
         <v>0.1399999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>-14.28941</v>
+      </c>
+      <c r="J10">
+        <v>-170.67959999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1">
         <v>68.287000000000006</v>
@@ -869,7 +892,7 @@
         <f>C11-B11</f>
         <v>1.6839999999999975</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="6">
         <v>1.76</v>
       </c>
@@ -880,10 +903,16 @@
         <f>G11-F11</f>
         <v>0.21999999999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>-14.28833</v>
+      </c>
+      <c r="J11">
+        <v>-170.67789999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1">
         <v>70.462000000000003</v>
@@ -895,7 +924,7 @@
         <f>C12-B12</f>
         <v>3.5219999999999914</v>
       </c>
-      <c r="E12" s="16"/>
+      <c r="E12" s="15"/>
       <c r="F12" s="6">
         <v>1.704</v>
       </c>
@@ -906,10 +935,16 @@
         <f>G12-F12</f>
         <v>1.0959999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>-14.29177</v>
+      </c>
+      <c r="J12">
+        <v>-170.68219999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
@@ -920,7 +955,7 @@
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="17"/>
+      <c r="E13" s="16"/>
       <c r="F13" s="6" t="s">
         <v>14</v>
       </c>
@@ -930,10 +965,16 @@
       <c r="H13" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>-14.29142</v>
+      </c>
+      <c r="J13">
+        <v>-170.67930000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1">
         <v>49.908999999999999</v>
@@ -945,7 +986,7 @@
         <f>C14-B14</f>
         <v>3.3980000000000032</v>
       </c>
-      <c r="E14" s="16"/>
+      <c r="E14" s="15"/>
       <c r="F14" s="6">
         <v>1.7290000000000001</v>
       </c>
@@ -956,22 +997,34 @@
         <f>G14-F14</f>
         <v>0.16799999999999993</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>-14.290330000000001</v>
+      </c>
+      <c r="J14">
+        <v>-170.67670000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="16"/>
+      <c r="E15" s="15"/>
       <c r="F15" s="6"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>-14.292730000000001</v>
+      </c>
+      <c r="J15">
+        <v>-170.67939999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>14</v>
@@ -982,7 +1035,7 @@
       <c r="D16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="17"/>
+      <c r="E16" s="16"/>
       <c r="F16" s="6" t="s">
         <v>14</v>
       </c>
@@ -992,10 +1045,16 @@
       <c r="H16" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>-14.293839999999999</v>
+      </c>
+      <c r="J16">
+        <v>-170.6773</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>14</v>
@@ -1006,7 +1065,7 @@
       <c r="D17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="17"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="6" t="s">
         <v>14</v>
       </c>
@@ -1016,18 +1075,24 @@
       <c r="H17" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>-14.293369999999999</v>
+      </c>
+      <c r="J17">
+        <v>-170.6754</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
-      <c r="E18" s="18"/>
+      <c r="E18" s="17"/>
       <c r="F18" s="12"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -1038,10 +1103,10 @@
         <v>78.757999999999996</v>
       </c>
       <c r="D19" s="4">
-        <f>C19-B19</f>
+        <f t="shared" ref="D19:D27" si="0">C19-B19</f>
         <v>9.070999999999998</v>
       </c>
-      <c r="E19" s="16"/>
+      <c r="E19" s="15"/>
       <c r="F19" s="6">
         <v>1.728</v>
       </c>
@@ -1049,11 +1114,17 @@
         <v>3.3410000000000002</v>
       </c>
       <c r="H19" s="1">
-        <f>G19-F19</f>
+        <f t="shared" ref="H19:H27" si="1">G19-F19</f>
         <v>1.6130000000000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>-14.290179999999999</v>
+      </c>
+      <c r="J19">
+        <v>-170.6814</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -1064,10 +1135,10 @@
         <v>110.946</v>
       </c>
       <c r="D20" s="4">
-        <f>C20-B20</f>
+        <f t="shared" si="0"/>
         <v>44.081999999999994</v>
       </c>
-      <c r="E20" s="16"/>
+      <c r="E20" s="15"/>
       <c r="F20" s="6">
         <v>1.6850000000000001</v>
       </c>
@@ -1075,11 +1146,17 @@
         <v>4.3150000000000004</v>
       </c>
       <c r="H20" s="1">
-        <f>G20-F20</f>
+        <f t="shared" si="1"/>
         <v>2.6300000000000003</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>-14.28941</v>
+      </c>
+      <c r="J20">
+        <v>-170.67959999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -1090,10 +1167,10 @@
         <v>106.504</v>
       </c>
       <c r="D21" s="4">
-        <f>C21-B21</f>
+        <f t="shared" si="0"/>
         <v>23.510000000000005</v>
       </c>
-      <c r="E21" s="16"/>
+      <c r="E21" s="15"/>
       <c r="F21" s="6">
         <v>1.722</v>
       </c>
@@ -1101,11 +1178,17 @@
         <v>3.597</v>
       </c>
       <c r="H21" s="1">
-        <f>G21-F21</f>
+        <f t="shared" si="1"/>
         <v>1.875</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>-14.28833</v>
+      </c>
+      <c r="J21">
+        <v>-170.67789999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -1116,10 +1199,10 @@
         <v>85.715000000000003</v>
       </c>
       <c r="D22" s="4">
-        <f>C22-B22</f>
+        <f t="shared" si="0"/>
         <v>15.51400000000001</v>
       </c>
-      <c r="E22" s="16"/>
+      <c r="E22" s="15"/>
       <c r="F22" s="6">
         <v>1.7809999999999999</v>
       </c>
@@ -1127,11 +1210,17 @@
         <v>4.3739999999999997</v>
       </c>
       <c r="H22" s="1">
-        <f>G22-F22</f>
+        <f t="shared" si="1"/>
         <v>2.593</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>-14.29177</v>
+      </c>
+      <c r="J22">
+        <v>-170.68219999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
@@ -1142,10 +1231,10 @@
         <v>73.19</v>
       </c>
       <c r="D23" s="4">
-        <f>C23-B23</f>
+        <f t="shared" si="0"/>
         <v>5.1239999999999952</v>
       </c>
-      <c r="E23" s="16"/>
+      <c r="E23" s="15"/>
       <c r="F23" s="6">
         <v>1.7330000000000001</v>
       </c>
@@ -1153,11 +1242,17 @@
         <v>3.3369</v>
       </c>
       <c r="H23" s="1">
-        <f>G23-F23</f>
+        <f t="shared" si="1"/>
         <v>1.6038999999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>-14.29142</v>
+      </c>
+      <c r="J23">
+        <v>-170.67930000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -1168,10 +1263,10 @@
         <v>89.942999999999998</v>
       </c>
       <c r="D24" s="4">
-        <f>C24-B24</f>
+        <f t="shared" si="0"/>
         <v>20.079999999999998</v>
       </c>
-      <c r="E24" s="16"/>
+      <c r="E24" s="15"/>
       <c r="F24" s="6">
         <v>1.734</v>
       </c>
@@ -1179,11 +1274,17 @@
         <v>2.9239999999999999</v>
       </c>
       <c r="H24" s="1">
-        <f>G24-F24</f>
+        <f t="shared" si="1"/>
         <v>1.19</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>-14.290330000000001</v>
+      </c>
+      <c r="J24">
+        <v>-170.67670000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>11</v>
       </c>
@@ -1194,10 +1295,10 @@
         <v>106.73099999999999</v>
       </c>
       <c r="D25" s="4">
-        <f>C25-B25</f>
+        <f t="shared" si="0"/>
         <v>39.299999999999997</v>
       </c>
-      <c r="E25" s="16"/>
+      <c r="E25" s="15"/>
       <c r="F25" s="6">
         <v>1.758</v>
       </c>
@@ -1205,11 +1306,17 @@
         <v>2.7690000000000001</v>
       </c>
       <c r="H25" s="1">
-        <f>G25-F25</f>
+        <f t="shared" si="1"/>
         <v>1.0110000000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>-14.292730000000001</v>
+      </c>
+      <c r="J25">
+        <v>-170.67939999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -1220,10 +1327,10 @@
         <v>99.766000000000005</v>
       </c>
       <c r="D26" s="4">
-        <f>C26-B26</f>
+        <f t="shared" si="0"/>
         <v>29.550000000000011</v>
       </c>
-      <c r="E26" s="16"/>
+      <c r="E26" s="15"/>
       <c r="F26" s="6">
         <v>1.6950000000000001</v>
       </c>
@@ -1231,11 +1338,17 @@
         <v>2.8730000000000002</v>
       </c>
       <c r="H26" s="1">
-        <f>G26-F26</f>
+        <f t="shared" si="1"/>
         <v>1.1780000000000002</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>-14.293839999999999</v>
+      </c>
+      <c r="J26">
+        <v>-170.6773</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
@@ -1246,10 +1359,10 @@
         <v>67.570999999999998</v>
       </c>
       <c r="D27" s="4">
-        <f>C27-B27</f>
+        <f t="shared" si="0"/>
         <v>1.2319999999999993</v>
       </c>
-      <c r="E27" s="16"/>
+      <c r="E27" s="15"/>
       <c r="F27" s="6">
         <v>1.746</v>
       </c>
@@ -1257,8 +1370,14 @@
         <v>2.9670000000000001</v>
       </c>
       <c r="H27" s="1">
-        <f>G27-F27</f>
+        <f t="shared" si="1"/>
         <v>1.2210000000000001</v>
+      </c>
+      <c r="I27">
+        <v>-14.293369999999999</v>
+      </c>
+      <c r="J27">
+        <v>-170.6754</v>
       </c>
     </row>
   </sheetData>
@@ -1280,10 +1399,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1298,25 +1417,28 @@
     <col min="8" max="8" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="9">
+        <v>41740</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="9">
+        <v>41777</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1324,30 +1446,30 @@
         <v>41806</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="F7" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="F7" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -1360,7 +1482,7 @@
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="5" t="s">
         <v>1</v>
       </c>
@@ -1370,10 +1492,16 @@
       <c r="H8" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1">
         <v>68.096800000000002</v>
@@ -1385,7 +1513,7 @@
         <f>C9-B9</f>
         <v>4.8465999999999951</v>
       </c>
-      <c r="E9" s="16"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="6">
         <v>1.7818000000000001</v>
       </c>
@@ -1396,10 +1524,16 @@
         <f>G9-F9</f>
         <v>0.12650000000000006</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>-14.290179999999999</v>
+      </c>
+      <c r="J9">
+        <v>-170.6814</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
@@ -1420,10 +1554,16 @@
       <c r="H10" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>-14.28941</v>
+      </c>
+      <c r="J10">
+        <v>-170.67959999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1">
         <v>67.465699999999998</v>
@@ -1435,7 +1575,7 @@
         <f>C11-B11</f>
         <v>0.12140000000000839</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="6">
         <v>1.7614000000000001</v>
       </c>
@@ -1446,10 +1586,16 @@
         <f>G11-F11</f>
         <v>-1.7400000000000082E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>-14.28833</v>
+      </c>
+      <c r="J11">
+        <v>-170.67789999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1">
         <v>70.368399999999994</v>
@@ -1461,7 +1607,7 @@
         <f>C12-B12</f>
         <v>4.0450000000000017</v>
       </c>
-      <c r="E12" s="16"/>
+      <c r="E12" s="15"/>
       <c r="F12" s="6">
         <v>1.7715000000000001</v>
       </c>
@@ -1472,10 +1618,16 @@
         <f>G12-F12</f>
         <v>0.52740000000000009</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>-14.29177</v>
+      </c>
+      <c r="J12">
+        <v>-170.68219999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1">
         <v>69.902000000000001</v>
@@ -1484,10 +1636,10 @@
         <v>70.447699999999998</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" ref="D13:D17" si="0">C13-B13</f>
+        <f t="shared" ref="D13:D16" si="0">C13-B13</f>
         <v>0.54569999999999652</v>
       </c>
-      <c r="E13" s="17"/>
+      <c r="E13" s="16"/>
       <c r="F13" s="6">
         <v>1.7643</v>
       </c>
@@ -1495,13 +1647,19 @@
         <v>1.7746999999999999</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" ref="H13:H17" si="1">G13-F13</f>
+        <f t="shared" ref="H13:H16" si="1">G13-F13</f>
         <v>1.0399999999999965E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>-14.29142</v>
+      </c>
+      <c r="J13">
+        <v>-170.67930000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1">
         <v>68.098600000000005</v>
@@ -1513,7 +1671,7 @@
         <f t="shared" si="0"/>
         <v>3.1409999999999911</v>
       </c>
-      <c r="E14" s="16"/>
+      <c r="E14" s="15"/>
       <c r="F14" s="6">
         <v>1.7568999999999999</v>
       </c>
@@ -1524,10 +1682,16 @@
         <f t="shared" si="1"/>
         <v>0.25150000000000006</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>-14.290330000000001</v>
+      </c>
+      <c r="J14">
+        <v>-170.67670000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1">
         <v>69.352199999999996</v>
@@ -1539,7 +1703,7 @@
         <f>C15-B15</f>
         <v>0.37330000000000041</v>
       </c>
-      <c r="E15" s="17"/>
+      <c r="E15" s="16"/>
       <c r="F15" s="6">
         <v>1.7564</v>
       </c>
@@ -1550,10 +1714,16 @@
         <f>G15-F15</f>
         <v>6.5999999999999392E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>-14.292730000000001</v>
+      </c>
+      <c r="J15">
+        <v>-170.67939999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1">
         <v>68.3232</v>
@@ -1565,7 +1735,7 @@
         <f t="shared" si="0"/>
         <v>2.030000000000598E-2</v>
       </c>
-      <c r="E16" s="17"/>
+      <c r="E16" s="16"/>
       <c r="F16" s="6">
         <v>1.7056</v>
       </c>
@@ -1576,10 +1746,16 @@
         <f t="shared" si="1"/>
         <v>1.2999999999999901E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>-14.293839999999999</v>
+      </c>
+      <c r="J16">
+        <v>-170.6773</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>14</v>
@@ -1600,18 +1776,24 @@
       <c r="H17" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>-14.293369999999999</v>
+      </c>
+      <c r="J17">
+        <v>-170.6754</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
-      <c r="E18" s="18"/>
+      <c r="E18" s="17"/>
       <c r="F18" s="12"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -1622,10 +1804,10 @@
         <v>69.556399999999996</v>
       </c>
       <c r="D19" s="4">
-        <f>C19-B19</f>
+        <f t="shared" ref="D19:D27" si="2">C19-B19</f>
         <v>2.0857000000000028</v>
       </c>
-      <c r="E19" s="16"/>
+      <c r="E19" s="15"/>
       <c r="F19" s="6">
         <v>1.7116</v>
       </c>
@@ -1633,11 +1815,17 @@
         <v>2.2997000000000001</v>
       </c>
       <c r="H19" s="1">
-        <f>G19-F19</f>
+        <f t="shared" ref="H19:H27" si="3">G19-F19</f>
         <v>0.58810000000000007</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>-14.290179999999999</v>
+      </c>
+      <c r="J19">
+        <v>-170.6814</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -1648,10 +1836,10 @@
         <v>85.320099999999996</v>
       </c>
       <c r="D20" s="4">
-        <f>C20-B20</f>
+        <f t="shared" si="2"/>
         <v>14.819400000000002</v>
       </c>
-      <c r="E20" s="16"/>
+      <c r="E20" s="15"/>
       <c r="F20" s="6">
         <v>1.7724</v>
       </c>
@@ -1659,11 +1847,17 @@
         <v>2.6053999999999999</v>
       </c>
       <c r="H20" s="1">
-        <f>G20-F20</f>
+        <f t="shared" si="3"/>
         <v>0.83299999999999996</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>-14.28941</v>
+      </c>
+      <c r="J20">
+        <v>-170.67959999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -1674,10 +1868,10 @@
         <v>74.888599999999997</v>
       </c>
       <c r="D21" s="4">
-        <f>C21-B21</f>
+        <f t="shared" si="2"/>
         <v>5.5343000000000018</v>
       </c>
-      <c r="E21" s="16"/>
+      <c r="E21" s="15"/>
       <c r="F21" s="6">
         <v>1.7591000000000001</v>
       </c>
@@ -1685,11 +1879,17 @@
         <v>3.1804999999999999</v>
       </c>
       <c r="H21" s="1">
-        <f>G21-F21</f>
+        <f t="shared" si="3"/>
         <v>1.4213999999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>-14.28833</v>
+      </c>
+      <c r="J21">
+        <v>-170.67789999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -1700,10 +1900,10 @@
         <v>72.950999999999993</v>
       </c>
       <c r="D22" s="4">
-        <f>C22-B22</f>
+        <f t="shared" si="2"/>
         <v>2.4510999999999967</v>
       </c>
-      <c r="E22" s="16"/>
+      <c r="E22" s="15"/>
       <c r="F22" s="6">
         <v>1.6861999999999999</v>
       </c>
@@ -1711,11 +1911,17 @@
         <v>3.0920999999999998</v>
       </c>
       <c r="H22" s="1">
-        <f>G22-F22</f>
+        <f t="shared" si="3"/>
         <v>1.4058999999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>-14.29177</v>
+      </c>
+      <c r="J22">
+        <v>-170.68219999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
@@ -1726,10 +1932,10 @@
         <v>70.768699999999995</v>
       </c>
       <c r="D23" s="4">
-        <f>C23-B23</f>
+        <f t="shared" si="2"/>
         <v>0.40009999999999479</v>
       </c>
-      <c r="E23" s="16"/>
+      <c r="E23" s="15"/>
       <c r="F23" s="6">
         <v>1.7655000000000001</v>
       </c>
@@ -1737,11 +1943,17 @@
         <v>1.9251</v>
       </c>
       <c r="H23" s="1">
-        <f>G23-F23</f>
+        <f t="shared" si="3"/>
         <v>0.15959999999999996</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>-14.29142</v>
+      </c>
+      <c r="J23">
+        <v>-170.67930000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -1752,10 +1964,10 @@
         <v>74.123800000000003</v>
       </c>
       <c r="D24" s="4">
-        <f>C24-B24</f>
+        <f t="shared" si="2"/>
         <v>7.0825999999999993</v>
       </c>
-      <c r="E24" s="16"/>
+      <c r="E24" s="15"/>
       <c r="F24" s="6">
         <v>1.6868000000000001</v>
       </c>
@@ -1763,11 +1975,17 @@
         <v>2.4535</v>
       </c>
       <c r="H24" s="1">
-        <f>G24-F24</f>
+        <f t="shared" si="3"/>
         <v>0.76669999999999994</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>-14.290330000000001</v>
+      </c>
+      <c r="J24">
+        <v>-170.67670000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>11</v>
       </c>
@@ -1778,10 +1996,10 @@
         <v>69.575400000000002</v>
       </c>
       <c r="D25" s="4">
-        <f>C25-B25</f>
+        <f t="shared" si="2"/>
         <v>1.2511999999999972</v>
       </c>
-      <c r="E25" s="16"/>
+      <c r="E25" s="15"/>
       <c r="F25" s="6">
         <v>1.7601</v>
       </c>
@@ -1789,11 +2007,17 @@
         <v>2.2749000000000001</v>
       </c>
       <c r="H25" s="1">
-        <f>G25-F25</f>
+        <f t="shared" si="3"/>
         <v>0.51480000000000015</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>-14.292730000000001</v>
+      </c>
+      <c r="J25">
+        <v>-170.67939999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -1804,10 +2028,10 @@
         <v>69.626800000000003</v>
       </c>
       <c r="D26" s="4">
-        <f>C26-B26</f>
+        <f t="shared" si="2"/>
         <v>1.5267000000000053</v>
       </c>
-      <c r="E26" s="16"/>
+      <c r="E26" s="15"/>
       <c r="F26" s="6">
         <v>1.7219</v>
       </c>
@@ -1815,11 +2039,17 @@
         <v>2.1839</v>
       </c>
       <c r="H26" s="1">
-        <f>G26-F26</f>
+        <f t="shared" si="3"/>
         <v>0.46199999999999997</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>-14.293839999999999</v>
+      </c>
+      <c r="J26">
+        <v>-170.6773</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
@@ -1830,10 +2060,10 @@
         <v>70.197699999999998</v>
       </c>
       <c r="D27" s="4">
-        <f>C27-B27</f>
+        <f t="shared" si="2"/>
         <v>0.29389999999999361</v>
       </c>
-      <c r="E27" s="16"/>
+      <c r="E27" s="15"/>
       <c r="F27" s="6">
         <v>1.7804</v>
       </c>
@@ -1841,8 +2071,14 @@
         <v>1.798</v>
       </c>
       <c r="H27" s="1">
-        <f>G27-F27</f>
+        <f t="shared" si="3"/>
         <v>1.760000000000006E-2</v>
+      </c>
+      <c r="I27">
+        <v>-14.293369999999999</v>
+      </c>
+      <c r="J27">
+        <v>-170.6754</v>
       </c>
     </row>
   </sheetData>
@@ -1861,10 +2097,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1879,56 +2115,59 @@
     <col min="8" max="8" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="9">
+        <v>41776</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="9">
+        <v>41816</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="F7" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="F7" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -1941,7 +2180,7 @@
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="5" t="s">
         <v>1</v>
       </c>
@@ -1951,10 +2190,16 @@
       <c r="H8" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1">
         <v>69.349999999999994</v>
@@ -1966,7 +2211,7 @@
         <f>C9-B9</f>
         <v>9.9100000000000108</v>
       </c>
-      <c r="E9" s="16"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="6">
         <v>1.77</v>
       </c>
@@ -1977,10 +2222,16 @@
         <f>G9-F9</f>
         <v>0.48999999999999977</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>-14.290179999999999</v>
+      </c>
+      <c r="J9">
+        <v>-170.6814</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1">
         <v>67.459999999999994</v>
@@ -1992,7 +2243,7 @@
         <f>C10-B10</f>
         <v>1.8200000000000074</v>
       </c>
-      <c r="E10" s="16"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="6">
         <v>1.75</v>
       </c>
@@ -2003,10 +2254,16 @@
         <f>G10-F10</f>
         <v>1.0000000000000009E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>-14.28941</v>
+      </c>
+      <c r="J10">
+        <v>-170.67959999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1">
         <v>68.319999999999993</v>
@@ -2018,7 +2275,7 @@
         <f>C11-B11</f>
         <v>2.4100000000000108</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="6">
         <v>1.79</v>
       </c>
@@ -2029,10 +2286,16 @@
         <f>G11-F11</f>
         <v>0.19999999999999996</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>-14.28833</v>
+      </c>
+      <c r="J11">
+        <v>-170.67789999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1">
         <v>67.040000000000006</v>
@@ -2044,7 +2307,7 @@
         <f>C12-B12</f>
         <v>4.2099999999999937</v>
       </c>
-      <c r="E12" s="16"/>
+      <c r="E12" s="15"/>
       <c r="F12" s="6">
         <v>1.74</v>
       </c>
@@ -2055,10 +2318,16 @@
         <f>G12-F12</f>
         <v>0.40999999999999992</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>-14.29177</v>
+      </c>
+      <c r="J12">
+        <v>-170.68219999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1">
         <v>70.5</v>
@@ -2070,7 +2339,7 @@
         <f t="shared" ref="D13:D17" si="0">C13-B13</f>
         <v>0.20000000000000284</v>
       </c>
-      <c r="E13" s="17"/>
+      <c r="E13" s="16"/>
       <c r="F13" s="6">
         <v>1.79</v>
       </c>
@@ -2081,10 +2350,16 @@
         <f t="shared" ref="H13:H17" si="1">G13-F13</f>
         <v>1.0000000000000009E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>-14.29142</v>
+      </c>
+      <c r="J13">
+        <v>-170.67930000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1">
         <v>69.900000000000006</v>
@@ -2096,7 +2371,7 @@
         <f t="shared" si="0"/>
         <v>0.36999999999999034</v>
       </c>
-      <c r="E14" s="16"/>
+      <c r="E14" s="15"/>
       <c r="F14" s="6">
         <v>1.77</v>
       </c>
@@ -2107,10 +2382,16 @@
         <f t="shared" si="1"/>
         <v>3.0000000000000027E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>-14.290330000000001</v>
+      </c>
+      <c r="J14">
+        <v>-170.67670000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1">
         <v>70.37</v>
@@ -2122,7 +2403,7 @@
         <f>C15-B15</f>
         <v>0.96999999999999886</v>
       </c>
-      <c r="E15" s="17"/>
+      <c r="E15" s="16"/>
       <c r="F15" s="6">
         <v>1.73</v>
       </c>
@@ -2133,10 +2414,16 @@
         <f>G15-F15</f>
         <v>0.24</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>-14.292730000000001</v>
+      </c>
+      <c r="J15">
+        <v>-170.67939999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1">
         <v>68.099999999999994</v>
@@ -2148,7 +2435,7 @@
         <f t="shared" si="0"/>
         <v>3.0000000000001137E-2</v>
       </c>
-      <c r="E16" s="17"/>
+      <c r="E16" s="16"/>
       <c r="F16" s="6">
         <v>1.75</v>
       </c>
@@ -2159,10 +2446,16 @@
         <f t="shared" si="1"/>
         <v>-7.0000000000000062E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>-14.293839999999999</v>
+      </c>
+      <c r="J16">
+        <v>-170.6773</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1">
         <v>67.459999999999994</v>
@@ -2174,7 +2467,7 @@
         <f t="shared" si="0"/>
         <v>-1.0699999999999932</v>
       </c>
-      <c r="E17" s="17"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="6">
         <v>1.68</v>
       </c>
@@ -2185,18 +2478,24 @@
         <f t="shared" si="1"/>
         <v>-7.9999999999999849E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>-14.293369999999999</v>
+      </c>
+      <c r="J17">
+        <v>-170.6754</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
-      <c r="E18" s="18"/>
+      <c r="E18" s="17"/>
       <c r="F18" s="12"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -2207,10 +2506,10 @@
         <v>71.819999999999993</v>
       </c>
       <c r="D19" s="4">
-        <f>C19-B19</f>
+        <f t="shared" ref="D19:D27" si="2">C19-B19</f>
         <v>5.4199999999999875</v>
       </c>
-      <c r="E19" s="16"/>
+      <c r="E19" s="15"/>
       <c r="F19" s="6">
         <v>1.71</v>
       </c>
@@ -2218,11 +2517,17 @@
         <v>2.04</v>
       </c>
       <c r="H19" s="1">
-        <f>G19-F19</f>
+        <f t="shared" ref="H19:H27" si="3">G19-F19</f>
         <v>0.33000000000000007</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>-14.290179999999999</v>
+      </c>
+      <c r="J19">
+        <v>-170.6814</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -2233,10 +2538,10 @@
         <v>85.83</v>
       </c>
       <c r="D20" s="4">
-        <f>C20-B20</f>
+        <f t="shared" si="2"/>
         <v>16.480000000000004</v>
       </c>
-      <c r="E20" s="16"/>
+      <c r="E20" s="15"/>
       <c r="F20" s="6">
         <v>1.81</v>
       </c>
@@ -2244,11 +2549,17 @@
         <v>2.38</v>
       </c>
       <c r="H20" s="1">
-        <f>G20-F20</f>
+        <f t="shared" si="3"/>
         <v>0.56999999999999984</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>-14.28941</v>
+      </c>
+      <c r="J20">
+        <v>-170.67959999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -2259,10 +2570,10 @@
         <v>79.510000000000005</v>
       </c>
       <c r="D21" s="4">
-        <f>C21-B21</f>
+        <f t="shared" si="2"/>
         <v>8.9400000000000119</v>
       </c>
-      <c r="E21" s="16"/>
+      <c r="E21" s="15"/>
       <c r="F21" s="6">
         <v>1.77</v>
       </c>
@@ -2270,11 +2581,17 @@
         <v>3.02</v>
       </c>
       <c r="H21" s="1">
-        <f>G21-F21</f>
+        <f t="shared" si="3"/>
         <v>1.25</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>-14.28833</v>
+      </c>
+      <c r="J21">
+        <v>-170.67789999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -2285,10 +2602,10 @@
         <v>69.849999999999994</v>
       </c>
       <c r="D22" s="4">
-        <f>C22-B22</f>
+        <f t="shared" si="2"/>
         <v>1.5300000000000011</v>
       </c>
-      <c r="E22" s="16"/>
+      <c r="E22" s="15"/>
       <c r="F22" s="6">
         <v>1.79</v>
       </c>
@@ -2296,11 +2613,17 @@
         <v>2.73</v>
       </c>
       <c r="H22" s="1">
-        <f>G22-F22</f>
+        <f t="shared" si="3"/>
         <v>0.94</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>-14.29177</v>
+      </c>
+      <c r="J22">
+        <v>-170.68219999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
@@ -2311,10 +2634,10 @@
         <v>70.510000000000005</v>
       </c>
       <c r="D23" s="4">
-        <f>C23-B23</f>
+        <f t="shared" si="2"/>
         <v>0.14000000000000057</v>
       </c>
-      <c r="E23" s="16"/>
+      <c r="E23" s="15"/>
       <c r="F23" s="6">
         <v>1.82</v>
       </c>
@@ -2322,11 +2645,17 @@
         <v>1.89</v>
       </c>
       <c r="H23" s="1">
-        <f>G23-F23</f>
+        <f t="shared" si="3"/>
         <v>6.999999999999984E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>-14.29142</v>
+      </c>
+      <c r="J23">
+        <v>-170.67930000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -2337,10 +2666,10 @@
         <v>77.48</v>
       </c>
       <c r="D24" s="4">
-        <f>C24-B24</f>
+        <f t="shared" si="2"/>
         <v>9.3800000000000097</v>
       </c>
-      <c r="E24" s="16"/>
+      <c r="E24" s="15"/>
       <c r="F24" s="6">
         <v>1.8</v>
       </c>
@@ -2348,11 +2677,17 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="H24" s="1">
-        <f>G24-F24</f>
+        <f t="shared" si="3"/>
         <v>0.49999999999999978</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>-14.290330000000001</v>
+      </c>
+      <c r="J24">
+        <v>-170.67670000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>11</v>
       </c>
@@ -2363,10 +2698,10 @@
         <v>72.86</v>
       </c>
       <c r="D25" s="4">
-        <f>C25-B25</f>
+        <f t="shared" si="2"/>
         <v>1.9599999999999937</v>
       </c>
-      <c r="E25" s="16"/>
+      <c r="E25" s="15"/>
       <c r="F25" s="6">
         <v>1.84</v>
       </c>
@@ -2374,11 +2709,17 @@
         <v>2.2200000000000002</v>
       </c>
       <c r="H25" s="1">
-        <f>G25-F25</f>
+        <f t="shared" si="3"/>
         <v>0.38000000000000012</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>-14.292730000000001</v>
+      </c>
+      <c r="J25">
+        <v>-170.67939999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -2389,10 +2730,10 @@
         <v>69.37</v>
       </c>
       <c r="D26" s="4">
-        <f>C26-B26</f>
+        <f t="shared" si="2"/>
         <v>2.3400000000000034</v>
       </c>
-      <c r="E26" s="16"/>
+      <c r="E26" s="15"/>
       <c r="F26" s="6">
         <v>1.76</v>
       </c>
@@ -2400,11 +2741,17 @@
         <v>2.21</v>
       </c>
       <c r="H26" s="1">
-        <f>G26-F26</f>
+        <f t="shared" si="3"/>
         <v>0.44999999999999996</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>-14.293839999999999</v>
+      </c>
+      <c r="J26">
+        <v>-170.6773</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
@@ -2415,10 +2762,10 @@
         <v>67.739999999999995</v>
       </c>
       <c r="D27" s="4">
-        <f>C27-B27</f>
+        <f t="shared" si="2"/>
         <v>0.28000000000000114</v>
       </c>
-      <c r="E27" s="16"/>
+      <c r="E27" s="15"/>
       <c r="F27" s="6">
         <v>1.79</v>
       </c>
@@ -2426,8 +2773,14 @@
         <v>1.9</v>
       </c>
       <c r="H27" s="1">
-        <f>G27-F27</f>
+        <f t="shared" si="3"/>
         <v>0.10999999999999988</v>
+      </c>
+      <c r="I27">
+        <v>-14.293369999999999</v>
+      </c>
+      <c r="J27">
+        <v>-170.6754</v>
       </c>
     </row>
   </sheetData>
@@ -2446,10 +2799,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2464,25 +2817,28 @@
     <col min="8" max="8" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="9">
+        <v>41816</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="9">
-        <v>41879</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>41865</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -2490,30 +2846,30 @@
         <v>41888</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="F7" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="F7" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -2526,7 +2882,7 @@
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="5" t="s">
         <v>1</v>
       </c>
@@ -2536,10 +2892,16 @@
       <c r="H8" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1">
         <v>70.497399999999999</v>
@@ -2551,7 +2913,7 @@
         <f>C9-B9</f>
         <v>12.896600000000007</v>
       </c>
-      <c r="E9" s="16"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="6">
         <v>1.7928999999999999</v>
       </c>
@@ -2562,34 +2924,46 @@
         <f>G9-F9</f>
         <v>0.46499999999999986</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>-14.290179999999999</v>
+      </c>
+      <c r="J9">
+        <v>-170.6814</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="16"/>
+        <v>24</v>
+      </c>
+      <c r="E10" s="15"/>
       <c r="F10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="I10">
+        <v>-14.28941</v>
+      </c>
+      <c r="J10">
+        <v>-170.67959999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1">
         <v>68.365799999999993</v>
@@ -2601,7 +2975,7 @@
         <f>C11-B11</f>
         <v>2.5868000000000109</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="6">
         <v>1.7181</v>
       </c>
@@ -2612,10 +2986,16 @@
         <f>G11-F11</f>
         <v>0.50129999999999986</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>-14.28833</v>
+      </c>
+      <c r="J11">
+        <v>-170.67789999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1">
         <v>69.883799999999994</v>
@@ -2627,7 +3007,7 @@
         <f>C12-B12</f>
         <v>8.9891000000000076</v>
       </c>
-      <c r="E12" s="16"/>
+      <c r="E12" s="15"/>
       <c r="F12" s="6">
         <v>1.7484</v>
       </c>
@@ -2638,10 +3018,16 @@
         <f>G12-F12</f>
         <v>1.6671000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>-14.29177</v>
+      </c>
+      <c r="J12">
+        <v>-170.68219999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1">
         <v>68.125699999999995</v>
@@ -2653,7 +3039,7 @@
         <f t="shared" ref="D13:D17" si="0">C13-B13</f>
         <v>0.32390000000000896</v>
       </c>
-      <c r="E13" s="17"/>
+      <c r="E13" s="16"/>
       <c r="F13" s="6">
         <v>1.7084999999999999</v>
       </c>
@@ -2664,10 +3050,16 @@
         <f t="shared" ref="H13:H17" si="1">G13-F13</f>
         <v>0.14100000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>-14.29142</v>
+      </c>
+      <c r="J13">
+        <v>-170.67930000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1">
         <v>67.0227</v>
@@ -2679,7 +3071,7 @@
         <f t="shared" si="0"/>
         <v>2.6208000000000027</v>
       </c>
-      <c r="E14" s="16"/>
+      <c r="E14" s="15"/>
       <c r="F14" s="6">
         <v>1.6861999999999999</v>
       </c>
@@ -2690,10 +3082,16 @@
         <f t="shared" si="1"/>
         <v>0.24250000000000016</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>-14.290330000000001</v>
+      </c>
+      <c r="J14">
+        <v>-170.67670000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1">
         <v>69.337100000000007</v>
@@ -2705,7 +3103,7 @@
         <f>C15-B15</f>
         <v>1.1396999999999906</v>
       </c>
-      <c r="E15" s="17"/>
+      <c r="E15" s="16"/>
       <c r="F15" s="6">
         <v>1.7007000000000001</v>
       </c>
@@ -2716,10 +3114,16 @@
         <f>G15-F15</f>
         <v>0.15479999999999983</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>-14.292730000000001</v>
+      </c>
+      <c r="J15">
+        <v>-170.67939999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1">
         <v>70.260000000000005</v>
@@ -2731,7 +3135,7 @@
         <f t="shared" si="0"/>
         <v>1.9899999999992701E-2</v>
       </c>
-      <c r="E16" s="17"/>
+      <c r="E16" s="16"/>
       <c r="F16" s="6">
         <v>1.7060999999999999</v>
       </c>
@@ -2742,10 +3146,16 @@
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>-14.293839999999999</v>
+      </c>
+      <c r="J16">
+        <v>-170.6773</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1">
         <v>67.492500000000007</v>
@@ -2757,7 +3167,7 @@
         <f t="shared" si="0"/>
         <v>8.5499999999996135E-2</v>
       </c>
-      <c r="E17" s="17"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="6">
         <v>1.7403</v>
       </c>
@@ -2768,18 +3178,24 @@
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>-14.293369999999999</v>
+      </c>
+      <c r="J17">
+        <v>-170.6754</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
-      <c r="E18" s="18"/>
+      <c r="E18" s="17"/>
       <c r="F18" s="12"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -2793,7 +3209,7 @@
         <f>C19-B19</f>
         <v>15.460300000000004</v>
       </c>
-      <c r="E19" s="16"/>
+      <c r="E19" s="15"/>
       <c r="F19" s="6">
         <v>1.7838000000000001</v>
       </c>
@@ -2804,8 +3220,14 @@
         <f>G19-F19</f>
         <v>1.4738999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>-14.290179999999999</v>
+      </c>
+      <c r="J19">
+        <v>-170.6814</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -2819,7 +3241,7 @@
         <f>C20-B20</f>
         <v>6.6499999999990678E-2</v>
       </c>
-      <c r="E20" s="16"/>
+      <c r="E20" s="15"/>
       <c r="F20" s="6">
         <v>1.7941</v>
       </c>
@@ -2830,8 +3252,14 @@
         <f>G20-F20</f>
         <v>-1.8000000000000016E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>-14.28941</v>
+      </c>
+      <c r="J20">
+        <v>-170.67959999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -2845,7 +3273,7 @@
         <f>C21-B21</f>
         <v>20.864499999999992</v>
       </c>
-      <c r="E21" s="16"/>
+      <c r="E21" s="15"/>
       <c r="F21" s="6">
         <v>1.732</v>
       </c>
@@ -2856,10 +3284,16 @@
         <f>G21-F21</f>
         <v>2.1639999999999997</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>-14.28833</v>
+      </c>
+      <c r="J21">
+        <v>-170.67789999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22" s="1">
         <v>66.432199999999995</v>
@@ -2871,7 +3305,7 @@
         <f>C22-B22</f>
         <v>19.016100000000009</v>
       </c>
-      <c r="E22" s="16"/>
+      <c r="E22" s="15"/>
       <c r="F22" s="6">
         <v>1.8023</v>
       </c>
@@ -2883,9 +3317,9 @@
         <v>1.0305000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B23" s="1">
         <v>69.380899999999997</v>
@@ -2897,7 +3331,7 @@
         <f t="shared" ref="D23:D26" si="2">C23-B23</f>
         <v>4.4121999999999986</v>
       </c>
-      <c r="E23" s="16"/>
+      <c r="E23" s="15"/>
       <c r="F23" s="6">
         <v>69.380899999999997</v>
       </c>
@@ -2909,9 +3343,9 @@
         <v>4.4121999999999986</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B24" s="1">
         <v>70.394800000000004</v>
@@ -2923,7 +3357,7 @@
         <f t="shared" si="2"/>
         <v>10.31519999999999</v>
       </c>
-      <c r="E24" s="16"/>
+      <c r="E24" s="15"/>
       <c r="F24" s="6">
         <v>1.6792</v>
       </c>
@@ -2935,9 +3369,9 @@
         <v>1.9421999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B25" s="1">
         <v>67.090900000000005</v>
@@ -2949,7 +3383,7 @@
         <f t="shared" si="2"/>
         <v>3.4407999999999959</v>
       </c>
-      <c r="E25" s="16"/>
+      <c r="E25" s="15"/>
       <c r="F25" s="6">
         <v>1.7887</v>
       </c>
@@ -2961,9 +3395,9 @@
         <v>2.2004999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26" s="1">
         <v>67.510959999999997</v>
@@ -2975,7 +3409,7 @@
         <f t="shared" si="2"/>
         <v>2.5642399999999981</v>
       </c>
-      <c r="E26" s="16"/>
+      <c r="E26" s="15"/>
       <c r="F26" s="6">
         <v>1.7210000000000001</v>
       </c>
@@ -2987,7 +3421,7 @@
         <v>3.2538999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
@@ -2997,15 +3431,21 @@
         <f>SUM(D22:D26)</f>
         <v>39.748539999999991</v>
       </c>
-      <c r="E27" s="16"/>
+      <c r="E27" s="15"/>
       <c r="F27" s="6"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1">
         <f>SUM(H22:H26)</f>
         <v>12.839299999999998</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>-14.29177</v>
+      </c>
+      <c r="J27">
+        <v>-170.68219999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
@@ -3019,7 +3459,7 @@
         <f>C28-B28</f>
         <v>5.1636999999999915</v>
       </c>
-      <c r="E28" s="16"/>
+      <c r="E28" s="15"/>
       <c r="F28" s="6">
         <v>1.7428999999999999</v>
       </c>
@@ -3030,8 +3470,14 @@
         <f>G28-F28</f>
         <v>1.5467000000000002</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>-14.29142</v>
+      </c>
+      <c r="J28">
+        <v>-170.67930000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
@@ -3045,7 +3491,7 @@
         <f>C29-B29</f>
         <v>16.414200000000008</v>
       </c>
-      <c r="E29" s="16"/>
+      <c r="E29" s="15"/>
       <c r="F29" s="6">
         <v>1.7764</v>
       </c>
@@ -3056,8 +3502,14 @@
         <f>G29-F29</f>
         <v>1.8008</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>-14.290330000000001</v>
+      </c>
+      <c r="J29">
+        <v>-170.67670000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>11</v>
       </c>
@@ -3071,7 +3523,7 @@
         <f>C30-B30</f>
         <v>15.743600000000001</v>
       </c>
-      <c r="E30" s="16"/>
+      <c r="E30" s="15"/>
       <c r="F30" s="6">
         <v>1.7115</v>
       </c>
@@ -3082,8 +3534,14 @@
         <f>G30-F30</f>
         <v>1.5703</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>-14.292730000000001</v>
+      </c>
+      <c r="J30">
+        <v>-170.67939999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
@@ -3097,7 +3555,7 @@
         <f>C31-B31</f>
         <v>10.990200000000002</v>
       </c>
-      <c r="E31" s="16"/>
+      <c r="E31" s="15"/>
       <c r="F31" s="6">
         <v>1.6805000000000001</v>
       </c>
@@ -3108,8 +3566,14 @@
         <f>G31-F31</f>
         <v>1.0395000000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>-14.293839999999999</v>
+      </c>
+      <c r="J31">
+        <v>-170.6773</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>12</v>
       </c>
@@ -3123,7 +3587,7 @@
         <f>C32-B32</f>
         <v>4.2900000000003047E-2</v>
       </c>
-      <c r="E32" s="16"/>
+      <c r="E32" s="15"/>
       <c r="F32" s="6">
         <v>1.73</v>
       </c>
@@ -3134,51 +3598,57 @@
         <f>G32-F32</f>
         <v>4.1500000000000092E-2</v>
       </c>
+      <c r="I32">
+        <v>-14.293369999999999</v>
+      </c>
+      <c r="J32">
+        <v>-170.6754</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3196,10 +3666,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3213,28 +3683,46 @@
     <col min="8" max="8" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="9">
+        <v>41865</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="9">
+        <v>41926</v>
+      </c>
+      <c r="H2">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="9">
         <v>41918</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="9">
+        <v>41926</v>
+      </c>
+      <c r="H3">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -3242,30 +3730,30 @@
         <v>41920</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="F7" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="F7" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -3288,532 +3776,803 @@
       <c r="H8" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1">
         <v>70.239999999999995</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1">
+        <v>96.644999999999996</v>
+      </c>
       <c r="D9" s="1">
         <f>C9-B9</f>
-        <v>-70.239999999999995</v>
-      </c>
-      <c r="E9" s="19" t="str">
+        <v>26.405000000000001</v>
+      </c>
+      <c r="E9" s="18" t="str">
         <f>A9</f>
         <v>P1A</v>
       </c>
       <c r="F9" s="1">
         <v>1.754</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1">
+        <v>4.7919999999999998</v>
+      </c>
       <c r="H9" s="1">
         <f>G9-F9</f>
-        <v>-1.754</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3.0379999999999998</v>
+      </c>
+      <c r="I9">
+        <v>-14.290179999999999</v>
+      </c>
+      <c r="J9">
+        <v>-170.6814</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="19" t="str">
-        <f t="shared" ref="E10:E21" si="0">A10</f>
+        <v>24</v>
+      </c>
+      <c r="E10" s="18" t="str">
+        <f t="shared" ref="E10:E33" si="0">A10</f>
         <v>P1B</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="I10">
+        <v>-14.28941</v>
+      </c>
+      <c r="J10">
+        <v>-170.67959999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B11" s="1">
         <v>68.073999999999998</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1">
+        <v>71.608999999999995</v>
+      </c>
       <c r="D11" s="1">
         <f>C11-B11</f>
-        <v>-68.073999999999998</v>
-      </c>
-      <c r="E11" s="19" t="str">
+        <v>3.5349999999999966</v>
+      </c>
+      <c r="E11" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>P1Ca</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1.754</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2.085</v>
+      </c>
+      <c r="H11" s="1">
+        <f>G11-F11</f>
+        <v>0.33099999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>P1Cb</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1.696</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" ref="H12:H17" si="1">G12-F12</f>
+        <v>0.60399999999999987</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>P1Cc</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1.7410000000000001</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1.792</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="1"/>
+        <v>5.0999999999999934E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1">
+        <f>B11</f>
+        <v>68.073999999999998</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" ref="C14:D14" si="2">C11</f>
+        <v>71.608999999999995</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="2"/>
+        <v>3.5349999999999966</v>
+      </c>
+      <c r="E14" s="18" t="str">
         <f t="shared" si="0"/>
         <v>P1C</v>
       </c>
-      <c r="F11" s="1">
-        <v>1.754</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1">
-        <f>G11-F11</f>
-        <v>-1.754</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="F14" s="1">
+        <f>SUM(F11:F13)</f>
+        <v>5.1910000000000007</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" ref="G14:H14" si="3">SUM(G11:G13)</f>
+        <v>6.1769999999999996</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="3"/>
+        <v>0.98599999999999977</v>
+      </c>
+      <c r="I14">
+        <v>-14.28833</v>
+      </c>
+      <c r="J14">
+        <v>-170.67789999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="1">
+        <v>69.646000000000001</v>
+      </c>
+      <c r="C15" s="1">
+        <v>72.480999999999995</v>
+      </c>
+      <c r="D15" s="1">
+        <f>C15-B15</f>
+        <v>2.8349999999999937</v>
+      </c>
+      <c r="E15" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>P2Aa</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1.746</v>
+      </c>
+      <c r="G15" s="1">
+        <v>3.4780000000000002</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="1"/>
+        <v>1.7320000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="19" t="str">
+      <c r="B16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>P1Cb</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1.696</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1">
-        <f t="shared" ref="H12:H16" si="1">G12-F12</f>
-        <v>-1.696</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+        <v>P2Ab</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1.74</v>
+      </c>
+      <c r="G16" s="1">
+        <v>4.0919999999999996</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="1"/>
+        <v>2.3519999999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="19" t="str">
+      <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>P1Cc</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1.7410000000000001</v>
-      </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1">
+        <v>P2Ac</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.671</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2.8450000000000002</v>
+      </c>
+      <c r="H17" s="1">
         <f t="shared" si="1"/>
-        <v>-1.7410000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="1">
+        <v>1.1740000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1">
+        <f>B15</f>
         <v>69.646000000000001</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1">
-        <f>C14-B14</f>
-        <v>-69.646000000000001</v>
-      </c>
-      <c r="E14" s="19" t="str">
+      <c r="C18" s="1">
+        <f t="shared" ref="C18:D18" si="4">C15</f>
+        <v>72.480999999999995</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="4"/>
+        <v>2.8349999999999937</v>
+      </c>
+      <c r="E18" s="18" t="str">
         <f t="shared" si="0"/>
         <v>P2A</v>
       </c>
-      <c r="F14" s="1">
-        <v>1.746</v>
-      </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.746</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>P2Ab</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1.74</v>
-      </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>P2Ac</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1.671</v>
-      </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.671</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="19" t="str">
+      <c r="F18" s="1">
+        <f>SUM(F15:F17)</f>
+        <v>5.157</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" ref="G18:H18" si="5">SUM(G15:G17)</f>
+        <v>10.415000000000001</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="5"/>
+        <v>5.258</v>
+      </c>
+      <c r="I18">
+        <v>-14.29177</v>
+      </c>
+      <c r="J18">
+        <v>-170.68219999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="18" t="str">
         <f t="shared" si="0"/>
         <v>P2B</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="1">
+      <c r="F19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19">
+        <v>-14.29142</v>
+      </c>
+      <c r="J19">
+        <v>-170.67930000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="1">
         <v>66.789000000000001</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1">
-        <f>C18-B18</f>
-        <v>-66.789000000000001</v>
-      </c>
-      <c r="E18" s="19" t="str">
+      <c r="C20" s="1">
+        <v>67.222999999999999</v>
+      </c>
+      <c r="D20" s="1">
+        <f>C20-B20</f>
+        <v>0.4339999999999975</v>
+      </c>
+      <c r="E20" s="18" t="str">
         <f t="shared" si="0"/>
         <v>P2C</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F20" s="1">
         <v>1.7490000000000001</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1">
-        <f>G18-F18</f>
-        <v>-1.7490000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="19" t="str">
+      <c r="G20" s="1">
+        <v>1.97</v>
+      </c>
+      <c r="H20" s="1">
+        <f>G20-F20</f>
+        <v>0.22099999999999986</v>
+      </c>
+      <c r="I20">
+        <v>-14.290330000000001</v>
+      </c>
+      <c r="J20">
+        <v>-170.67670000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="18" t="str">
         <f t="shared" si="0"/>
         <v>P3A</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="19" t="str">
+      <c r="F21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21">
+        <v>-14.292730000000001</v>
+      </c>
+      <c r="J21">
+        <v>-170.67939999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="18" t="str">
         <f t="shared" si="0"/>
         <v>P3B</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="1">
+      <c r="F22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22">
+        <v>-14.293839999999999</v>
+      </c>
+      <c r="J22">
+        <v>-170.6773</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="1">
         <v>67.215999999999994</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1">
-        <f t="shared" ref="D21" si="2">C21-B21</f>
-        <v>-67.215999999999994</v>
-      </c>
-      <c r="E21" s="19" t="str">
+      <c r="C23" s="1">
+        <v>67.221000000000004</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" ref="D23" si="6">C23-B23</f>
+        <v>5.0000000000096634E-3</v>
+      </c>
+      <c r="E23" s="18" t="str">
         <f t="shared" si="0"/>
         <v>P3C</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F23" s="1">
         <v>1.746</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1">
-        <f t="shared" ref="H21" si="3">G21-F21</f>
-        <v>-1.746</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="G23" s="1">
+        <v>1.7250000000000001</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" ref="H23" si="7">G23-F23</f>
+        <v>-2.0999999999999908E-2</v>
+      </c>
+      <c r="I23">
+        <v>-14.293369999999999</v>
+      </c>
+      <c r="J23">
+        <v>-170.6754</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B25" s="1">
         <v>67.849999999999994</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1">
-        <f t="shared" ref="D23:D31" si="4">C23-B23</f>
-        <v>-67.849999999999994</v>
-      </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="1">
+      <c r="C25" s="1">
+        <v>72.977000000000004</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" ref="D25:D33" si="8">C25-B25</f>
+        <v>5.1270000000000095</v>
+      </c>
+      <c r="E25" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>T1A</v>
+      </c>
+      <c r="F25" s="1">
         <v>1.7809999999999999</v>
       </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1">
-        <f t="shared" ref="H23:H31" si="5">G23-F23</f>
-        <v>-1.7809999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="G25" s="1">
+        <v>7.6020000000000003</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" ref="H25:H33" si="9">G25-F25</f>
+        <v>5.8210000000000006</v>
+      </c>
+      <c r="I25">
+        <v>-14.290179999999999</v>
+      </c>
+      <c r="J25">
+        <v>-170.6814</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="B26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>T1B</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26">
+        <v>-14.28941</v>
+      </c>
+      <c r="J26">
+        <v>-170.67959999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B27" s="1">
         <v>66.135000000000005</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1">
-        <f t="shared" si="4"/>
-        <v>-66.135000000000005</v>
-      </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="1">
+      <c r="C27" s="1">
+        <v>66.171000000000006</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="8"/>
+        <v>3.6000000000001364E-2</v>
+      </c>
+      <c r="E27" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>T1C</v>
+      </c>
+      <c r="F27" s="1">
         <v>1.7290000000000001</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1">
-        <f t="shared" si="5"/>
-        <v>-1.7290000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="G27" s="1">
+        <v>16.518000000000001</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="9"/>
+        <v>14.789000000000001</v>
+      </c>
+      <c r="I27">
+        <v>-14.28833</v>
+      </c>
+      <c r="J27">
+        <v>-170.67789999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B28" s="1">
         <v>70.003</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1">
-        <f t="shared" si="4"/>
-        <v>-70.003</v>
-      </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="1">
+      <c r="C28" s="1">
+        <v>70.637</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="8"/>
+        <v>0.63400000000000034</v>
+      </c>
+      <c r="E28" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>T2A</v>
+      </c>
+      <c r="F28" s="1">
         <v>1.7470000000000001</v>
       </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1">
-        <f t="shared" si="5"/>
-        <v>-1.7470000000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="G28" s="1">
+        <v>11.294</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="9"/>
+        <v>9.5470000000000006</v>
+      </c>
+      <c r="I28">
+        <v>-14.29177</v>
+      </c>
+      <c r="J28">
+        <v>-170.68219999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="1">
+      <c r="B29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>T2B</v>
+      </c>
+      <c r="F29" s="1">
         <v>1.736</v>
       </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1">
-        <f t="shared" si="5"/>
-        <v>-1.736</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="G29" s="1">
+        <f>1.976</f>
+        <v>1.976</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="9"/>
+        <v>0.24</v>
+      </c>
+      <c r="I29">
+        <v>-14.29142</v>
+      </c>
+      <c r="J29">
+        <v>-170.67930000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="1">
+      <c r="B30" s="1">
+        <v>69.093999999999994</v>
+      </c>
+      <c r="C30" s="1">
+        <v>72.986999999999995</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="8"/>
+        <v>3.8930000000000007</v>
+      </c>
+      <c r="E30" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>T2C</v>
+      </c>
+      <c r="F30" s="1">
         <v>1.677</v>
       </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1">
-        <f t="shared" si="5"/>
-        <v>-1.677</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="G30" s="1">
+        <v>11.345000000000001</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="9"/>
+        <v>9.668000000000001</v>
+      </c>
+      <c r="I30">
+        <v>-14.290330000000001</v>
+      </c>
+      <c r="J30">
+        <v>-170.67670000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B31" s="1">
         <v>112.001</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1">
-        <f t="shared" si="4"/>
-        <v>-112.001</v>
-      </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="1">
+      <c r="C31" s="1">
+        <v>114.126</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="8"/>
+        <v>2.125</v>
+      </c>
+      <c r="E31" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>T3A</v>
+      </c>
+      <c r="F31" s="1">
         <v>1.6930000000000001</v>
       </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1">
-        <f t="shared" si="5"/>
-        <v>-1.6930000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="G31" s="1">
+        <v>5.1719999999999997</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="9"/>
+        <v>3.4789999999999996</v>
+      </c>
+      <c r="I31">
+        <v>-14.292730000000001</v>
+      </c>
+      <c r="J31">
+        <v>-170.67939999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B32" s="1">
         <v>112.91800000000001</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1">
-        <f t="shared" si="4"/>
-        <v>-112.91800000000001</v>
-      </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="1">
+      <c r="C32" s="1">
+        <v>118.40300000000001</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="8"/>
+        <v>5.4849999999999994</v>
+      </c>
+      <c r="E32" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>T3B</v>
+      </c>
+      <c r="F32" s="1">
         <v>1.774</v>
       </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1">
-        <f t="shared" si="5"/>
-        <v>-1.774</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="G32" s="1">
+        <v>3.6930000000000001</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="9"/>
+        <v>1.919</v>
+      </c>
+      <c r="I32">
+        <v>-14.293839999999999</v>
+      </c>
+      <c r="J32">
+        <v>-170.6773</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B33" s="1">
         <v>70.108000000000004</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1">
-        <f t="shared" si="4"/>
-        <v>-70.108000000000004</v>
-      </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="1">
+      <c r="C33" s="1">
+        <v>70.945999999999998</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="8"/>
+        <v>0.83799999999999386</v>
+      </c>
+      <c r="E33" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>T3C</v>
+      </c>
+      <c r="F33" s="1">
         <v>1.7390000000000001</v>
       </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1">
-        <f t="shared" si="5"/>
-        <v>-1.7390000000000001</v>
+      <c r="G33" s="1">
+        <v>3.3420000000000001</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="9"/>
+        <v>1.603</v>
+      </c>
+      <c r="I33">
+        <v>-14.293369999999999</v>
+      </c>
+      <c r="J33">
+        <v>-170.6754</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed to g/m2/day to match other literature
</commit_message>
<xml_diff>
--- a/Data/BulkWeight/SedPod_Processing_LAB.xlsx
+++ b/Data/BulkWeight/SedPod_Processing_LAB.xlsx
@@ -19,7 +19,6 @@
     <sheet name="Aug_Sept" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -197,9 +196,6 @@
     <t>Days deployed:</t>
   </si>
   <si>
-    <t>Area(cm2)</t>
-  </si>
-  <si>
     <t>SedPod radius=</t>
   </si>
   <si>
@@ -207,12 +203,19 @@
   </si>
   <si>
     <t xml:space="preserve">SedTube radius = </t>
+  </si>
+  <si>
+    <t>Area(m2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -331,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -358,7 +361,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="L27" sqref="L19:L27"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8:L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -768,18 +772,18 @@
         <v>37</v>
       </c>
       <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2">
+        <f>3*0.0254</f>
+        <v>7.619999999999999E-2</v>
+      </c>
+      <c r="H2" t="s">
         <v>58</v>
-      </c>
-      <c r="G2">
-        <f>3*2.54</f>
-        <v>7.62</v>
-      </c>
-      <c r="H2" t="s">
-        <v>59</v>
       </c>
       <c r="I2" s="22">
         <f>PI()*G2^2</f>
-        <v>182.41469247509917</v>
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -790,18 +794,18 @@
         <v>41740</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G3">
-        <f>2*2.54</f>
-        <v>5.08</v>
+        <f>2*0.0254</f>
+        <v>5.0799999999999998E-2</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="22">
+        <v>58</v>
+      </c>
+      <c r="I3" s="23">
         <f>PI()*G3^2</f>
-        <v>81.073196655599631</v>
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -868,7 +872,7 @@
         <v>56</v>
       </c>
       <c r="L8" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -906,8 +910,8 @@
         <f>$B$3-$B$2</f>
         <v>37</v>
       </c>
-      <c r="L9">
-        <v>182.4</v>
+      <c r="L9" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -945,8 +949,8 @@
         <f t="shared" ref="K10:K27" si="0">$B$3-$B$2</f>
         <v>37</v>
       </c>
-      <c r="L10">
-        <v>182.4</v>
+      <c r="L10" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -984,8 +988,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L11">
-        <v>182.4</v>
+      <c r="L11" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1023,8 +1027,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L12">
-        <v>182.4</v>
+      <c r="L12" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1060,8 +1064,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L13">
-        <v>182.4</v>
+      <c r="L13" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1099,8 +1103,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L14">
-        <v>182.4</v>
+      <c r="L14" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1124,8 +1128,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L15">
-        <v>182.4</v>
+      <c r="L15" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1161,8 +1165,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L16">
-        <v>182.4</v>
+      <c r="L16" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1198,8 +1202,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L17">
-        <v>182.4</v>
+      <c r="L17" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1247,8 +1251,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L19">
-        <v>81</v>
+      <c r="L19" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1286,8 +1290,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L20">
-        <v>81</v>
+      <c r="L20" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1325,8 +1329,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L21">
-        <v>81</v>
+      <c r="L21" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1364,8 +1368,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L22">
-        <v>81</v>
+      <c r="L22" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1403,8 +1407,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L23">
-        <v>81</v>
+      <c r="L23" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1442,8 +1446,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L24">
-        <v>81</v>
+      <c r="L24" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1481,8 +1485,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L25">
-        <v>81</v>
+      <c r="L25" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1520,8 +1524,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L26">
-        <v>81</v>
+      <c r="L26" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1559,8 +1563,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L27">
-        <v>81</v>
+      <c r="L27" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1579,8 +1583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19:L27"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8:L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1687,7 +1691,7 @@
         <v>56</v>
       </c>
       <c r="L8" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1725,8 +1729,8 @@
         <f t="shared" ref="K9:K27" si="0">$B$3-$B$2</f>
         <v>37</v>
       </c>
-      <c r="L9">
-        <v>182.4</v>
+      <c r="L9" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1762,8 +1766,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L10">
-        <v>182.4</v>
+      <c r="L10" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1801,8 +1805,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L11">
-        <v>182.4</v>
+      <c r="L11" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1840,8 +1844,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L12">
-        <v>182.4</v>
+      <c r="L12" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1879,8 +1883,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L13">
-        <v>182.4</v>
+      <c r="L13" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1918,8 +1922,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L14">
-        <v>182.4</v>
+      <c r="L14" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1957,8 +1961,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L15">
-        <v>182.4</v>
+      <c r="L15" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1996,8 +2000,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L16">
-        <v>182.4</v>
+      <c r="L16" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2033,8 +2037,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L17">
-        <v>182.4</v>
+      <c r="L17" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2082,8 +2086,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L19">
-        <v>81</v>
+      <c r="L19" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2121,8 +2125,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L20">
-        <v>81</v>
+      <c r="L20" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2160,8 +2164,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L21">
-        <v>81</v>
+      <c r="L21" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2199,8 +2203,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L22">
-        <v>81</v>
+      <c r="L22" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2238,8 +2242,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L23">
-        <v>81</v>
+      <c r="L23" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2277,8 +2281,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L24">
-        <v>81</v>
+      <c r="L24" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2316,8 +2320,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L25">
-        <v>81</v>
+      <c r="L25" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2355,8 +2359,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L26">
-        <v>81</v>
+      <c r="L26" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2394,8 +2398,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L27">
-        <v>81</v>
+      <c r="L27" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
   </sheetData>
@@ -2416,8 +2420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19:L27"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8:L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2524,7 +2528,7 @@
         <v>56</v>
       </c>
       <c r="L8" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2562,8 +2566,8 @@
         <f t="shared" ref="K9:K27" si="2">$B$3-$B$2</f>
         <v>40</v>
       </c>
-      <c r="L9">
-        <v>182.4</v>
+      <c r="L9" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -2601,8 +2605,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L10">
-        <v>182.4</v>
+      <c r="L10" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2640,8 +2644,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L11">
-        <v>182.4</v>
+      <c r="L11" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2679,8 +2683,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L12">
-        <v>182.4</v>
+      <c r="L12" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2718,8 +2722,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L13">
-        <v>182.4</v>
+      <c r="L13" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2757,8 +2761,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L14">
-        <v>182.4</v>
+      <c r="L14" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2796,8 +2800,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L15">
-        <v>182.4</v>
+      <c r="L15" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2835,8 +2839,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L16">
-        <v>182.4</v>
+      <c r="L16" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2874,8 +2878,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L17">
-        <v>182.4</v>
+      <c r="L17" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2923,8 +2927,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L19">
-        <v>81</v>
+      <c r="L19" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2962,8 +2966,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L20">
-        <v>81</v>
+      <c r="L20" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -3001,8 +3005,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L21">
-        <v>81</v>
+      <c r="L21" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -3040,8 +3044,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L22">
-        <v>81</v>
+      <c r="L22" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -3079,8 +3083,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L23">
-        <v>81</v>
+      <c r="L23" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -3118,8 +3122,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L24">
-        <v>81</v>
+      <c r="L24" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -3157,8 +3161,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L25">
-        <v>81</v>
+      <c r="L25" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -3196,8 +3200,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L26">
-        <v>81</v>
+      <c r="L26" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -3235,8 +3239,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L27">
-        <v>81</v>
+      <c r="L27" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
   </sheetData>
@@ -3257,8 +3261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8:L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3365,7 +3369,7 @@
         <v>56</v>
       </c>
       <c r="L8" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3403,8 +3407,8 @@
         <f t="shared" ref="K9:K17" si="0">$B$3-$B$2</f>
         <v>49</v>
       </c>
-      <c r="L9">
-        <v>182.4</v>
+      <c r="L9" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -3440,8 +3444,8 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="L10">
-        <v>182.4</v>
+      <c r="L10" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -3479,8 +3483,8 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="L11">
-        <v>182.4</v>
+      <c r="L11" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3518,8 +3522,8 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="L12">
-        <v>182.4</v>
+      <c r="L12" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -3557,8 +3561,8 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="L13">
-        <v>182.4</v>
+      <c r="L13" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -3596,8 +3600,8 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="L14">
-        <v>182.4</v>
+      <c r="L14" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -3635,8 +3639,8 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="L15">
-        <v>182.4</v>
+      <c r="L15" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -3673,8 +3677,8 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="L16">
-        <v>182.4</v>
+      <c r="L16" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -3711,8 +3715,8 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="L17">
-        <v>182.4</v>
+      <c r="L17" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3760,8 +3764,8 @@
         <f t="shared" ref="K19:K21" si="5">$B$3-$B$2</f>
         <v>49</v>
       </c>
-      <c r="L19">
-        <v>81</v>
+      <c r="L19" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -3799,8 +3803,8 @@
         <f t="shared" si="5"/>
         <v>49</v>
       </c>
-      <c r="L20">
-        <v>81</v>
+      <c r="L20" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -3838,8 +3842,8 @@
         <f t="shared" si="5"/>
         <v>49</v>
       </c>
-      <c r="L21">
-        <v>81</v>
+      <c r="L21" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -3867,6 +3871,7 @@
         <f t="shared" si="4"/>
         <v>1.0305000000000002</v>
       </c>
+      <c r="L22" s="22"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -3893,6 +3898,7 @@
         <f t="shared" si="4"/>
         <v>4.4121999999999986</v>
       </c>
+      <c r="L23" s="22"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -3919,6 +3925,7 @@
         <f t="shared" si="4"/>
         <v>1.9421999999999999</v>
       </c>
+      <c r="L24" s="22"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -3945,6 +3952,7 @@
         <f t="shared" si="4"/>
         <v>2.2004999999999999</v>
       </c>
+      <c r="L25" s="22"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -3971,6 +3979,7 @@
         <f t="shared" si="4"/>
         <v>3.2538999999999998</v>
       </c>
+      <c r="L26" s="22"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -3999,8 +4008,8 @@
         <f t="shared" ref="K27:K32" si="6">$B$3-$B$2</f>
         <v>49</v>
       </c>
-      <c r="L27">
-        <v>81</v>
+      <c r="L27" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -4038,8 +4047,8 @@
         <f t="shared" si="6"/>
         <v>49</v>
       </c>
-      <c r="L28">
-        <v>81</v>
+      <c r="L28" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -4077,8 +4086,8 @@
         <f t="shared" si="6"/>
         <v>49</v>
       </c>
-      <c r="L29">
-        <v>81</v>
+      <c r="L29" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -4116,8 +4125,8 @@
         <f t="shared" si="6"/>
         <v>49</v>
       </c>
-      <c r="L30">
-        <v>81</v>
+      <c r="L30" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -4155,8 +4164,8 @@
         <f t="shared" si="6"/>
         <v>49</v>
       </c>
-      <c r="L31">
-        <v>81</v>
+      <c r="L31" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -4194,8 +4203,8 @@
         <f t="shared" si="6"/>
         <v>49</v>
       </c>
-      <c r="L32">
-        <v>81</v>
+      <c r="L32" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -4261,8 +4270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4386,7 +4395,7 @@
         <v>56</v>
       </c>
       <c r="L8" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -4427,8 +4436,8 @@
         <f t="shared" ref="K9:K10" si="0">$B$3-$B$2</f>
         <v>53</v>
       </c>
-      <c r="L9">
-        <v>182.4</v>
+      <c r="L9" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -4467,8 +4476,8 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="L10">
-        <v>182.4</v>
+      <c r="L10" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -4499,6 +4508,7 @@
         <f>G11-F11</f>
         <v>0.33099999999999996</v>
       </c>
+      <c r="L11" s="22"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -4523,6 +4533,7 @@
         <f t="shared" ref="H12:H17" si="2">G12-F12</f>
         <v>0.60399999999999987</v>
       </c>
+      <c r="L12" s="22"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -4547,6 +4558,7 @@
         <f t="shared" si="2"/>
         <v>5.0999999999999934E-2</v>
       </c>
+      <c r="L13" s="22"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -4590,8 +4602,8 @@
         <f t="shared" ref="K14" si="3">$B$3-$B$2</f>
         <v>53</v>
       </c>
-      <c r="L14">
-        <v>182.4</v>
+      <c r="L14" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -4622,6 +4634,7 @@
         <f t="shared" si="2"/>
         <v>1.7320000000000002</v>
       </c>
+      <c r="L15" s="22"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -4646,6 +4659,7 @@
         <f t="shared" si="2"/>
         <v>2.3519999999999994</v>
       </c>
+      <c r="L16" s="22"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -4670,6 +4684,7 @@
         <f t="shared" si="2"/>
         <v>1.1740000000000002</v>
       </c>
+      <c r="L17" s="22"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -4713,8 +4728,8 @@
         <f t="shared" ref="K18:K23" si="4">$B$3-$B$2</f>
         <v>53</v>
       </c>
-      <c r="L18">
-        <v>182.4</v>
+      <c r="L18" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -4753,8 +4768,8 @@
         <f t="shared" si="4"/>
         <v>53</v>
       </c>
-      <c r="L19">
-        <v>182.4</v>
+      <c r="L19" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -4795,8 +4810,8 @@
         <f t="shared" si="4"/>
         <v>53</v>
       </c>
-      <c r="L20">
-        <v>182.4</v>
+      <c r="L20" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -4835,8 +4850,8 @@
         <f t="shared" si="4"/>
         <v>53</v>
       </c>
-      <c r="L21">
-        <v>182.4</v>
+      <c r="L21" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -4875,8 +4890,8 @@
         <f t="shared" si="4"/>
         <v>53</v>
       </c>
-      <c r="L22">
-        <v>182.4</v>
+      <c r="L22" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -4917,8 +4932,8 @@
         <f t="shared" si="4"/>
         <v>53</v>
       </c>
-      <c r="L23">
-        <v>182.4</v>
+      <c r="L23" s="22">
+        <v>1.8241469247509915E-2</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4969,8 +4984,8 @@
         <f t="shared" ref="K25:K33" si="7">$B$3-$B$2</f>
         <v>53</v>
       </c>
-      <c r="L25">
-        <v>81</v>
+      <c r="L25" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -5009,8 +5024,8 @@
         <f t="shared" si="7"/>
         <v>53</v>
       </c>
-      <c r="L26">
-        <v>81</v>
+      <c r="L26" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -5051,8 +5066,8 @@
         <f t="shared" si="7"/>
         <v>53</v>
       </c>
-      <c r="L27">
-        <v>81</v>
+      <c r="L27" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -5093,8 +5108,8 @@
         <f t="shared" si="7"/>
         <v>53</v>
       </c>
-      <c r="L28">
-        <v>81</v>
+      <c r="L28" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -5135,8 +5150,8 @@
         <f t="shared" si="7"/>
         <v>53</v>
       </c>
-      <c r="L29">
-        <v>81</v>
+      <c r="L29" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -5177,8 +5192,8 @@
         <f t="shared" si="7"/>
         <v>53</v>
       </c>
-      <c r="L30">
-        <v>81</v>
+      <c r="L30" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -5219,8 +5234,8 @@
         <f t="shared" si="7"/>
         <v>53</v>
       </c>
-      <c r="L31">
-        <v>81</v>
+      <c r="L31" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -5261,8 +5276,8 @@
         <f t="shared" si="7"/>
         <v>53</v>
       </c>
-      <c r="L32">
-        <v>81</v>
+      <c r="L32" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -5303,8 +5318,8 @@
         <f t="shared" si="7"/>
         <v>53</v>
       </c>
-      <c r="L33">
-        <v>81</v>
+      <c r="L33" s="22">
+        <v>8.107319665559963E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed radius of tube traps to 1in
it was using the diameter of 2in.
added some lit values for coral stress
</commit_message>
<xml_diff>
--- a/Data/BulkWeight/SedPod_Processing_LAB.xlsx
+++ b/Data/BulkWeight/SedPod_Processing_LAB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Mar" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="Jun_Jul" sheetId="6" r:id="rId4"/>
     <sheet name="Aug_Sept" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="63">
   <si>
     <t>Pod(P)/Tube(T)</t>
   </si>
@@ -206,15 +206,20 @@
   </si>
   <si>
     <t>Area(m2)</t>
+  </si>
+  <si>
+    <t>(marked 5/16/14 on bags)</t>
+  </si>
+  <si>
+    <t>(marked 7/1/14 on bags)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="167" formatCode="0.000000"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -334,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -358,11 +363,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8:L27"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -781,8 +785,8 @@
       <c r="H2" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="22">
-        <f>PI()*G2^2</f>
+      <c r="I2" s="21">
+        <f>PI()*(G2^2)</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -797,15 +801,15 @@
         <v>59</v>
       </c>
       <c r="G3">
-        <f>2*0.0254</f>
-        <v>5.0799999999999998E-2</v>
+        <f>1*0.0254</f>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="H3" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="23">
-        <f>PI()*G3^2</f>
-        <v>8.107319665559963E-3</v>
+      <c r="I3" s="21">
+        <f>PI()*(G3^2)</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -828,16 +832,16 @@
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="F7" s="21" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="F7" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -910,7 +914,8 @@
         <f>$B$3-$B$2</f>
         <v>37</v>
       </c>
-      <c r="L9" s="22">
+      <c r="L9" s="21">
+        <f>$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -949,7 +954,8 @@
         <f t="shared" ref="K10:K27" si="0">$B$3-$B$2</f>
         <v>37</v>
       </c>
-      <c r="L10" s="22">
+      <c r="L10" s="21">
+        <f t="shared" ref="L10:L17" si="1">$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -988,7 +994,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L11" s="22">
+      <c r="L11" s="21">
+        <f t="shared" si="1"/>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -1027,7 +1034,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L12" s="22">
+      <c r="L12" s="21">
+        <f t="shared" si="1"/>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -1064,7 +1072,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="21">
+        <f t="shared" si="1"/>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -1103,7 +1112,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="21">
+        <f t="shared" si="1"/>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -1128,7 +1138,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="21">
+        <f t="shared" si="1"/>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -1165,7 +1176,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L16" s="22">
+      <c r="L16" s="21">
+        <f t="shared" si="1"/>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -1202,7 +1214,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L17" s="22">
+      <c r="L17" s="21">
+        <f t="shared" si="1"/>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -1227,7 +1240,7 @@
         <v>78.757999999999996</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" ref="D19:D27" si="1">C19-B19</f>
+        <f t="shared" ref="D19:D27" si="2">C19-B19</f>
         <v>9.070999999999998</v>
       </c>
       <c r="E19" s="15"/>
@@ -1238,7 +1251,7 @@
         <v>3.3410000000000002</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" ref="H19:H27" si="2">G19-F19</f>
+        <f t="shared" ref="H19:H27" si="3">G19-F19</f>
         <v>1.6130000000000002</v>
       </c>
       <c r="I19">
@@ -1251,8 +1264,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L19" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L19" s="21">
+        <f>$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1266,7 +1280,7 @@
         <v>110.946</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44.081999999999994</v>
       </c>
       <c r="E20" s="15"/>
@@ -1277,7 +1291,7 @@
         <v>4.3150000000000004</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.6300000000000003</v>
       </c>
       <c r="I20">
@@ -1290,8 +1304,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L20" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L20" s="21">
+        <f t="shared" ref="L20:L27" si="4">$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1305,7 +1320,7 @@
         <v>106.504</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23.510000000000005</v>
       </c>
       <c r="E21" s="15"/>
@@ -1316,7 +1331,7 @@
         <v>3.597</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.875</v>
       </c>
       <c r="I21">
@@ -1329,8 +1344,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L21" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L21" s="21">
+        <f t="shared" si="4"/>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1344,7 +1360,7 @@
         <v>85.715000000000003</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15.51400000000001</v>
       </c>
       <c r="E22" s="15"/>
@@ -1355,7 +1371,7 @@
         <v>4.3739999999999997</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.593</v>
       </c>
       <c r="I22">
@@ -1368,8 +1384,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L22" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L22" s="21">
+        <f t="shared" si="4"/>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1383,7 +1400,7 @@
         <v>73.19</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.1239999999999952</v>
       </c>
       <c r="E23" s="15"/>
@@ -1394,7 +1411,7 @@
         <v>3.3369</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.6038999999999999</v>
       </c>
       <c r="I23">
@@ -1407,8 +1424,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L23" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L23" s="21">
+        <f t="shared" si="4"/>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1422,7 +1440,7 @@
         <v>89.942999999999998</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20.079999999999998</v>
       </c>
       <c r="E24" s="15"/>
@@ -1433,7 +1451,7 @@
         <v>2.9239999999999999</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.19</v>
       </c>
       <c r="I24">
@@ -1446,8 +1464,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L24" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L24" s="21">
+        <f t="shared" si="4"/>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1461,7 +1480,7 @@
         <v>106.73099999999999</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39.299999999999997</v>
       </c>
       <c r="E25" s="15"/>
@@ -1472,7 +1491,7 @@
         <v>2.7690000000000001</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0110000000000001</v>
       </c>
       <c r="I25">
@@ -1485,8 +1504,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L25" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L25" s="21">
+        <f t="shared" si="4"/>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1500,7 +1520,7 @@
         <v>99.766000000000005</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29.550000000000011</v>
       </c>
       <c r="E26" s="15"/>
@@ -1511,7 +1531,7 @@
         <v>2.8730000000000002</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1780000000000002</v>
       </c>
       <c r="I26">
@@ -1524,8 +1544,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L26" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L26" s="21">
+        <f t="shared" si="4"/>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1539,7 +1560,7 @@
         <v>67.570999999999998</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2319999999999993</v>
       </c>
       <c r="E27" s="15"/>
@@ -1550,7 +1571,7 @@
         <v>2.9670000000000001</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2210000000000001</v>
       </c>
       <c r="I27">
@@ -1563,8 +1584,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L27" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L27" s="21">
+        <f t="shared" si="4"/>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1583,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8:L27"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L19" activeCellId="1" sqref="L9 L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1626,6 +1648,9 @@
       <c r="B3" s="9">
         <v>41777</v>
       </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1647,16 +1672,16 @@
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="F7" s="21" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="F7" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1729,7 +1754,8 @@
         <f t="shared" ref="K9:K27" si="0">$B$3-$B$2</f>
         <v>37</v>
       </c>
-      <c r="L9" s="22">
+      <c r="L9" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -1766,7 +1792,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L10" s="22">
+      <c r="L10" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -1805,7 +1832,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L11" s="22">
+      <c r="L11" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -1844,7 +1872,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L12" s="22">
+      <c r="L12" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -1883,7 +1912,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -1922,7 +1952,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -1961,7 +1992,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -2000,7 +2032,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L16" s="22">
+      <c r="L16" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -2037,7 +2070,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L17" s="22">
+      <c r="L17" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -2086,8 +2120,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L19" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L19" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2125,8 +2160,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L20" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L20" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2164,8 +2200,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L21" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L21" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2203,8 +2240,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L22" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L22" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2242,8 +2280,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L23" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L23" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2281,8 +2320,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L24" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L24" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2320,8 +2360,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L25" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L25" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2359,8 +2400,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L26" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L26" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2398,8 +2440,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L27" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L27" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
   </sheetData>
@@ -2420,8 +2463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8:L27"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2463,6 +2506,9 @@
       <c r="B3" s="9">
         <v>41816</v>
       </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2484,16 +2530,16 @@
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="F7" s="21" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="F7" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -2566,7 +2612,8 @@
         <f t="shared" ref="K9:K27" si="2">$B$3-$B$2</f>
         <v>40</v>
       </c>
-      <c r="L9" s="22">
+      <c r="L9" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -2605,7 +2652,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L10" s="22">
+      <c r="L10" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -2644,7 +2692,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L11" s="22">
+      <c r="L11" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -2683,7 +2732,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L12" s="22">
+      <c r="L12" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -2722,7 +2772,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -2761,7 +2812,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -2800,7 +2852,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -2839,7 +2892,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L16" s="22">
+      <c r="L16" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -2878,7 +2932,8 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L17" s="22">
+      <c r="L17" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -2927,8 +2982,9 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L19" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L19" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2966,8 +3022,9 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L20" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L20" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -3005,8 +3062,9 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L21" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L21" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -3044,8 +3102,9 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L22" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L22" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -3083,8 +3142,9 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L23" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L23" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -3122,8 +3182,9 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L24" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L24" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -3161,8 +3222,9 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L25" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L25" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -3200,8 +3262,9 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L26" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L26" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -3239,8 +3302,9 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="L27" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L27" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
   </sheetData>
@@ -3261,8 +3325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8:L32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3325,16 +3389,16 @@
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="F7" s="21" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="F7" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -3407,7 +3471,8 @@
         <f t="shared" ref="K9:K17" si="0">$B$3-$B$2</f>
         <v>49</v>
       </c>
-      <c r="L9" s="22">
+      <c r="L9" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -3444,7 +3509,8 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="L10" s="22">
+      <c r="L10" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -3483,7 +3549,8 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="L11" s="22">
+      <c r="L11" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -3522,7 +3589,8 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="L12" s="22">
+      <c r="L12" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -3561,7 +3629,8 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -3600,7 +3669,8 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -3639,7 +3709,8 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -3677,7 +3748,8 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="L16" s="22">
+      <c r="L16" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -3715,7 +3787,8 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="L17" s="22">
+      <c r="L17" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -3764,8 +3837,9 @@
         <f t="shared" ref="K19:K21" si="5">$B$3-$B$2</f>
         <v>49</v>
       </c>
-      <c r="L19" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L19" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -3803,8 +3877,9 @@
         <f t="shared" si="5"/>
         <v>49</v>
       </c>
-      <c r="L20" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L20" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -3842,8 +3917,9 @@
         <f t="shared" si="5"/>
         <v>49</v>
       </c>
-      <c r="L21" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L21" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -3871,7 +3947,7 @@
         <f t="shared" si="4"/>
         <v>1.0305000000000002</v>
       </c>
-      <c r="L22" s="22"/>
+      <c r="L22" s="21"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -3898,7 +3974,7 @@
         <f t="shared" si="4"/>
         <v>4.4121999999999986</v>
       </c>
-      <c r="L23" s="22"/>
+      <c r="L23" s="21"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -3925,7 +4001,7 @@
         <f t="shared" si="4"/>
         <v>1.9421999999999999</v>
       </c>
-      <c r="L24" s="22"/>
+      <c r="L24" s="21"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -3952,7 +4028,7 @@
         <f t="shared" si="4"/>
         <v>2.2004999999999999</v>
       </c>
-      <c r="L25" s="22"/>
+      <c r="L25" s="21"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -3979,7 +4055,7 @@
         <f t="shared" si="4"/>
         <v>3.2538999999999998</v>
       </c>
-      <c r="L26" s="22"/>
+      <c r="L26" s="21"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -4008,8 +4084,9 @@
         <f t="shared" ref="K27:K32" si="6">$B$3-$B$2</f>
         <v>49</v>
       </c>
-      <c r="L27" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L27" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -4047,8 +4124,9 @@
         <f t="shared" si="6"/>
         <v>49</v>
       </c>
-      <c r="L28" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L28" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -4086,8 +4164,9 @@
         <f t="shared" si="6"/>
         <v>49</v>
       </c>
-      <c r="L29" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L29" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -4125,8 +4204,9 @@
         <f t="shared" si="6"/>
         <v>49</v>
       </c>
-      <c r="L30" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L30" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -4164,8 +4244,9 @@
         <f t="shared" si="6"/>
         <v>49</v>
       </c>
-      <c r="L31" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L31" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -4203,8 +4284,9 @@
         <f t="shared" si="6"/>
         <v>49</v>
       </c>
-      <c r="L32" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L32" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -4270,8 +4352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView topLeftCell="A4" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25:L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4351,16 +4433,16 @@
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="F7" s="21" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="F7" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -4436,7 +4518,8 @@
         <f t="shared" ref="K9:K10" si="0">$B$3-$B$2</f>
         <v>53</v>
       </c>
-      <c r="L9" s="22">
+      <c r="L9" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -4476,7 +4559,8 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="L10" s="22">
+      <c r="L10" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -4508,7 +4592,7 @@
         <f>G11-F11</f>
         <v>0.33099999999999996</v>
       </c>
-      <c r="L11" s="22"/>
+      <c r="L11" s="21"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -4533,7 +4617,7 @@
         <f t="shared" ref="H12:H17" si="2">G12-F12</f>
         <v>0.60399999999999987</v>
       </c>
-      <c r="L12" s="22"/>
+      <c r="L12" s="21"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -4558,7 +4642,7 @@
         <f t="shared" si="2"/>
         <v>5.0999999999999934E-2</v>
       </c>
-      <c r="L13" s="22"/>
+      <c r="L13" s="21"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -4602,7 +4686,8 @@
         <f t="shared" ref="K14" si="3">$B$3-$B$2</f>
         <v>53</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -4634,7 +4719,7 @@
         <f t="shared" si="2"/>
         <v>1.7320000000000002</v>
       </c>
-      <c r="L15" s="22"/>
+      <c r="L15" s="21"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -4659,7 +4744,7 @@
         <f t="shared" si="2"/>
         <v>2.3519999999999994</v>
       </c>
-      <c r="L16" s="22"/>
+      <c r="L16" s="21"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -4684,7 +4769,7 @@
         <f t="shared" si="2"/>
         <v>1.1740000000000002</v>
       </c>
-      <c r="L17" s="22"/>
+      <c r="L17" s="21"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -4728,7 +4813,8 @@
         <f t="shared" ref="K18:K23" si="4">$B$3-$B$2</f>
         <v>53</v>
       </c>
-      <c r="L18" s="22">
+      <c r="L18" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -4768,7 +4854,8 @@
         <f t="shared" si="4"/>
         <v>53</v>
       </c>
-      <c r="L19" s="22">
+      <c r="L19" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -4810,7 +4897,8 @@
         <f t="shared" si="4"/>
         <v>53</v>
       </c>
-      <c r="L20" s="22">
+      <c r="L20" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -4850,7 +4938,8 @@
         <f t="shared" si="4"/>
         <v>53</v>
       </c>
-      <c r="L21" s="22">
+      <c r="L21" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -4890,7 +4979,8 @@
         <f t="shared" si="4"/>
         <v>53</v>
       </c>
-      <c r="L22" s="22">
+      <c r="L22" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -4932,7 +5022,8 @@
         <f t="shared" si="4"/>
         <v>53</v>
       </c>
-      <c r="L23" s="22">
+      <c r="L23" s="21">
+        <f>Mar!$I$2</f>
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
@@ -4984,8 +5075,9 @@
         <f t="shared" ref="K25:K33" si="7">$B$3-$B$2</f>
         <v>53</v>
       </c>
-      <c r="L25" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L25" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -5024,8 +5116,9 @@
         <f t="shared" si="7"/>
         <v>53</v>
       </c>
-      <c r="L26" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L26" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -5066,8 +5159,9 @@
         <f t="shared" si="7"/>
         <v>53</v>
       </c>
-      <c r="L27" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L27" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -5108,8 +5202,9 @@
         <f t="shared" si="7"/>
         <v>53</v>
       </c>
-      <c r="L28" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L28" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -5150,8 +5245,9 @@
         <f t="shared" si="7"/>
         <v>53</v>
       </c>
-      <c r="L29" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L29" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -5192,8 +5288,9 @@
         <f t="shared" si="7"/>
         <v>53</v>
       </c>
-      <c r="L30" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L30" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -5234,8 +5331,9 @@
         <f t="shared" si="7"/>
         <v>53</v>
       </c>
-      <c r="L31" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L31" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -5276,8 +5374,9 @@
         <f t="shared" si="7"/>
         <v>53</v>
       </c>
-      <c r="L32" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L32" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -5318,8 +5417,9 @@
         <f t="shared" si="7"/>
         <v>53</v>
       </c>
-      <c r="L33" s="22">
-        <v>8.107319665559963E-3</v>
+      <c r="L33" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
November sample collection started
</commit_message>
<xml_diff>
--- a/Data/BulkWeight/SedPod_Processing_LAB.xlsx
+++ b/Data/BulkWeight/SedPod_Processing_LAB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Mar" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="May" sheetId="4" r:id="rId3"/>
     <sheet name="Jun_Jul" sheetId="6" r:id="rId4"/>
     <sheet name="Aug_Sept" sheetId="3" r:id="rId5"/>
+    <sheet name="Oct" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="64">
   <si>
     <t>Pod(P)/Tube(T)</t>
   </si>
@@ -212,6 +213,9 @@
   </si>
   <si>
     <t>(marked 7/1/14 on bags)</t>
+  </si>
+  <si>
+    <t>Messina, Curtis</t>
   </si>
 </sst>
 </file>
@@ -3325,7 +3329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -4352,7 +4356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="L25" sqref="L25:L33"/>
     </sheetView>
   </sheetViews>
@@ -5432,4 +5436,859 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="16.625" customWidth="1"/>
+    <col min="3" max="3" width="20.375" customWidth="1"/>
+    <col min="4" max="4" width="17.375" customWidth="1"/>
+    <col min="5" max="5" width="7.375" customWidth="1"/>
+    <col min="6" max="6" width="14.875" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="18.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="9">
+        <v>41918</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2">
+        <f>B3-B2</f>
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="9">
+        <v>41926</v>
+      </c>
+      <c r="H2">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="9">
+        <v>41953</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="9">
+        <v>41926</v>
+      </c>
+      <c r="H3">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="9">
+        <v>41955</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="F7" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1">
+        <v>70.239000000000004</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1">
+        <f>C9-B9</f>
+        <v>-70.239000000000004</v>
+      </c>
+      <c r="E9" s="18" t="str">
+        <f>A9</f>
+        <v>P1A</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1.742</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1">
+        <f>G9-F9</f>
+        <v>-1.742</v>
+      </c>
+      <c r="I9">
+        <v>-14.290179999999999</v>
+      </c>
+      <c r="J9">
+        <v>-170.6814</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ref="K9:K10" si="0">$B$3-$B$2</f>
+        <v>35</v>
+      </c>
+      <c r="L9" s="21">
+        <f>Mar!$I$2</f>
+        <v>1.8241469247509915E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1">
+        <v>109.636</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1">
+        <f t="shared" ref="D10:D17" si="1">C10-B10</f>
+        <v>-109.636</v>
+      </c>
+      <c r="E10" s="18" t="str">
+        <f t="shared" ref="E10:E27" si="2">A10</f>
+        <v>P1B</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1.7170000000000001</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1">
+        <f t="shared" ref="H10:H17" si="3">G10-F10</f>
+        <v>-1.7170000000000001</v>
+      </c>
+      <c r="I10">
+        <v>-14.28941</v>
+      </c>
+      <c r="J10">
+        <v>-170.67959999999999</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="L10" s="21">
+        <f>Mar!$I$2</f>
+        <v>1.8241469247509915E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1">
+        <v>68.070999999999998</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1">
+        <f t="shared" si="1"/>
+        <v>-68.070999999999998</v>
+      </c>
+      <c r="E11" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>P1C</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.8</v>
+      </c>
+      <c r="I11">
+        <v>-14.28833</v>
+      </c>
+      <c r="J11">
+        <v>-170.67789999999999</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ref="K11" si="4">$B$3-$B$2</f>
+        <v>35</v>
+      </c>
+      <c r="L11" s="21">
+        <f>Mar!$I$2</f>
+        <v>1.8241469247509915E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1">
+        <v>69.646000000000001</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1">
+        <f t="shared" si="1"/>
+        <v>-69.646000000000001</v>
+      </c>
+      <c r="E12" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>P2A</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1.7130000000000001</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.7130000000000001</v>
+      </c>
+      <c r="I12">
+        <v>-14.29177</v>
+      </c>
+      <c r="J12">
+        <v>-170.68219999999999</v>
+      </c>
+      <c r="K12">
+        <f t="shared" ref="K12:K17" si="5">$B$3-$B$2</f>
+        <v>35</v>
+      </c>
+      <c r="L12" s="21">
+        <f>Mar!$I$2</f>
+        <v>1.8241469247509915E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1">
+        <v>112.90600000000001</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1">
+        <f t="shared" si="1"/>
+        <v>-112.90600000000001</v>
+      </c>
+      <c r="E13" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>P2B</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1.7330000000000001</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.7330000000000001</v>
+      </c>
+      <c r="I13">
+        <v>-14.29142</v>
+      </c>
+      <c r="J13">
+        <v>-170.67930000000001</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="L13" s="21">
+        <f>Mar!$I$2</f>
+        <v>1.8241469247509915E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1">
+        <v>66.784999999999997</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1">
+        <f t="shared" si="1"/>
+        <v>-66.784999999999997</v>
+      </c>
+      <c r="E14" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>P2C</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1.7869999999999999</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.7869999999999999</v>
+      </c>
+      <c r="I14">
+        <v>-14.290330000000001</v>
+      </c>
+      <c r="J14">
+        <v>-170.67670000000001</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="L14" s="21">
+        <f>Mar!$I$2</f>
+        <v>1.8241469247509915E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1">
+        <v>114.151</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1">
+        <f t="shared" si="1"/>
+        <v>-114.151</v>
+      </c>
+      <c r="E15" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>P3A</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1.7410000000000001</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.7410000000000001</v>
+      </c>
+      <c r="I15">
+        <v>-14.292730000000001</v>
+      </c>
+      <c r="J15">
+        <v>-170.67939999999999</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="L15" s="21">
+        <f>Mar!$I$2</f>
+        <v>1.8241469247509915E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>P3B</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16">
+        <v>-14.293839999999999</v>
+      </c>
+      <c r="J16">
+        <v>-170.6773</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="L16" s="21">
+        <f>Mar!$I$2</f>
+        <v>1.8241469247509915E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="1">
+        <v>67.215999999999994</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1">
+        <f t="shared" si="1"/>
+        <v>-67.215999999999994</v>
+      </c>
+      <c r="E17" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>P3C</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.7529999999999999</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.7529999999999999</v>
+      </c>
+      <c r="I17">
+        <v>-14.293369999999999</v>
+      </c>
+      <c r="J17">
+        <v>-170.6754</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="L17" s="21">
+        <f>Mar!$I$2</f>
+        <v>1.8241469247509915E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1">
+        <v>67.875</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1">
+        <f t="shared" ref="D19:D27" si="6">C19-B19</f>
+        <v>-67.875</v>
+      </c>
+      <c r="E19" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>T1A</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1.7410000000000001</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1">
+        <f t="shared" ref="H19:H27" si="7">G19-F19</f>
+        <v>-1.7410000000000001</v>
+      </c>
+      <c r="I19">
+        <v>-14.290179999999999</v>
+      </c>
+      <c r="J19">
+        <v>-170.6814</v>
+      </c>
+      <c r="K19">
+        <f t="shared" ref="K19:K27" si="8">$B$3-$B$2</f>
+        <v>35</v>
+      </c>
+      <c r="L19" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="1">
+        <v>111.997</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1">
+        <f t="shared" si="6"/>
+        <v>-111.997</v>
+      </c>
+      <c r="E20" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>T1B</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1.704</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.704</v>
+      </c>
+      <c r="I20">
+        <v>-14.28941</v>
+      </c>
+      <c r="J20">
+        <v>-170.67959999999999</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+      <c r="L20" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1">
+        <v>66.126000000000005</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1">
+        <f t="shared" si="6"/>
+        <v>-66.126000000000005</v>
+      </c>
+      <c r="E21" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>T1C</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1.754</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.754</v>
+      </c>
+      <c r="I21">
+        <v>-14.28833</v>
+      </c>
+      <c r="J21">
+        <v>-170.67789999999999</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+      <c r="L21" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="1">
+        <v>70.001000000000005</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1">
+        <f t="shared" si="6"/>
+        <v>-70.001000000000005</v>
+      </c>
+      <c r="E22" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>T2A</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1.81</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.81</v>
+      </c>
+      <c r="I22">
+        <v>-14.29177</v>
+      </c>
+      <c r="J22">
+        <v>-170.68219999999999</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+      <c r="L22" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="1">
+        <v>114.664</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1">
+        <f t="shared" si="6"/>
+        <v>-114.664</v>
+      </c>
+      <c r="E23" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>T2B</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1.7370000000000001</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.7370000000000001</v>
+      </c>
+      <c r="I23">
+        <v>-14.29142</v>
+      </c>
+      <c r="J23">
+        <v>-170.67930000000001</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+      <c r="L23" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="1">
+        <v>69.096000000000004</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1">
+        <f t="shared" si="6"/>
+        <v>-69.096000000000004</v>
+      </c>
+      <c r="E24" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>T2C</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1.7190000000000001</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.7190000000000001</v>
+      </c>
+      <c r="I24">
+        <v>-14.290330000000001</v>
+      </c>
+      <c r="J24">
+        <v>-170.67670000000001</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+      <c r="L24" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="1">
+        <v>112.929</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1">
+        <f t="shared" si="6"/>
+        <v>-112.929</v>
+      </c>
+      <c r="E25" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>T3A</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1.796</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.796</v>
+      </c>
+      <c r="I25">
+        <v>-14.292730000000001</v>
+      </c>
+      <c r="J25">
+        <v>-170.67939999999999</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+      <c r="L25" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="1">
+        <v>112.92</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1">
+        <f t="shared" si="6"/>
+        <v>-112.92</v>
+      </c>
+      <c r="E26" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>T3B</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1.8109999999999999</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.8109999999999999</v>
+      </c>
+      <c r="I26">
+        <v>-14.293839999999999</v>
+      </c>
+      <c r="J26">
+        <v>-170.6773</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+      <c r="L26" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="1">
+        <v>70.11</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1">
+        <f t="shared" si="6"/>
+        <v>-70.11</v>
+      </c>
+      <c r="E27" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>T3C</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1.7989999999999999</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.7989999999999999</v>
+      </c>
+      <c r="I27">
+        <v>-14.293369999999999</v>
+      </c>
+      <c r="J27">
+        <v>-170.6754</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+      <c r="L27" s="21">
+        <f>Mar!$I$3</f>
+        <v>2.0268299163899908E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="F7:H7"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>